<commit_message>
final tarea viernes 13/06. detalle en mail miercoles 18/06.
</commit_message>
<xml_diff>
--- a/data/CENSO_salud.xlsX
+++ b/data/CENSO_salud.xlsX
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\research_migration\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83A639E-550C-4571-A9FA-C8047D218F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B69BA5-7E42-451D-9FD6-489E6C8D041F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28695" yWindow="15" windowWidth="14610" windowHeight="15585" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Output" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja2" sheetId="4" r:id="rId3"/>
-    <sheet name="Hoja3" sheetId="5" r:id="rId4"/>
-    <sheet name="Hoja4" sheetId="6" r:id="rId5"/>
+    <sheet name="Migrante" sheetId="2" r:id="rId2"/>
+    <sheet name="arg1" sheetId="4" r:id="rId3"/>
+    <sheet name="arg2" sheetId="5" r:id="rId4"/>
+    <sheet name="total" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -274,9 +274,6 @@
     <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -287,6 +284,9 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -598,7 +598,7 @@
   </sheetPr>
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A22" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
       <selection activeCell="C30" sqref="C30:F34"/>
     </sheetView>
   </sheetViews>
@@ -614,182 +614,182 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
     </row>
     <row r="2" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
     </row>
     <row r="3" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
     </row>
     <row r="4" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
     </row>
     <row r="5" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
     </row>
     <row r="6" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
     </row>
     <row r="7" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
     </row>
     <row r="8" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
     </row>
     <row r="9" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
     </row>
     <row r="10" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
     </row>
     <row r="11" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
     </row>
     <row r="12" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
     </row>
     <row r="13" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
@@ -812,11 +812,11 @@
       <c r="C14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
       <c r="G14" s="4"/>
       <c r="H14" s="5"/>
       <c r="I14" s="2"/>
@@ -825,7 +825,7 @@
     </row>
     <row r="15" spans="1:11" ht="14.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="16" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="1"/>
@@ -846,7 +846,7 @@
     </row>
     <row r="16" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
-      <c r="B16" s="12"/>
+      <c r="B16" s="16"/>
       <c r="C16" s="1" t="s">
         <v>18</v>
       </c>
@@ -867,7 +867,7 @@
     </row>
     <row r="17" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
-      <c r="B17" s="12"/>
+      <c r="B17" s="16"/>
       <c r="C17" s="1" t="s">
         <v>19</v>
       </c>
@@ -888,7 +888,7 @@
     </row>
     <row r="18" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
-      <c r="B18" s="12"/>
+      <c r="B18" s="16"/>
       <c r="C18" s="1" t="s">
         <v>20</v>
       </c>
@@ -909,7 +909,7 @@
     </row>
     <row r="19" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
-      <c r="B19" s="12"/>
+      <c r="B19" s="16"/>
       <c r="C19" s="10" t="s">
         <v>21</v>
       </c>
@@ -930,7 +930,7 @@
     </row>
     <row r="20" spans="1:11" ht="14.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="16" t="s">
         <v>22</v>
       </c>
       <c r="C20" s="1"/>
@@ -951,7 +951,7 @@
     </row>
     <row r="21" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
-      <c r="B21" s="12"/>
+      <c r="B21" s="16"/>
       <c r="C21" s="1" t="s">
         <v>18</v>
       </c>
@@ -972,7 +972,7 @@
     </row>
     <row r="22" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
-      <c r="B22" s="12"/>
+      <c r="B22" s="16"/>
       <c r="C22" s="1" t="s">
         <v>19</v>
       </c>
@@ -993,7 +993,7 @@
     </row>
     <row r="23" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
-      <c r="B23" s="12"/>
+      <c r="B23" s="16"/>
       <c r="C23" s="1" t="s">
         <v>20</v>
       </c>
@@ -1014,7 +1014,7 @@
     </row>
     <row r="24" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
-      <c r="B24" s="12"/>
+      <c r="B24" s="16"/>
       <c r="C24" s="10" t="s">
         <v>21</v>
       </c>
@@ -1035,7 +1035,7 @@
     </row>
     <row r="25" spans="1:11" ht="14.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="1"/>
@@ -1056,7 +1056,7 @@
     </row>
     <row r="26" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
-      <c r="B26" s="12"/>
+      <c r="B26" s="16"/>
       <c r="C26" s="1" t="s">
         <v>18</v>
       </c>
@@ -1077,7 +1077,7 @@
     </row>
     <row r="27" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
-      <c r="B27" s="12"/>
+      <c r="B27" s="16"/>
       <c r="C27" s="1" t="s">
         <v>19</v>
       </c>
@@ -1098,7 +1098,7 @@
     </row>
     <row r="28" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
-      <c r="B28" s="12"/>
+      <c r="B28" s="16"/>
       <c r="C28" s="1" t="s">
         <v>20</v>
       </c>
@@ -1119,7 +1119,7 @@
     </row>
     <row r="29" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
-      <c r="B29" s="12"/>
+      <c r="B29" s="16"/>
       <c r="C29" s="10" t="s">
         <v>21</v>
       </c>
@@ -1140,7 +1140,7 @@
     </row>
     <row r="30" spans="1:11" ht="14.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="16" t="s">
         <v>17</v>
       </c>
       <c r="C30" s="1"/>
@@ -1161,7 +1161,7 @@
     </row>
     <row r="31" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
-      <c r="B31" s="12"/>
+      <c r="B31" s="16"/>
       <c r="C31" s="1" t="s">
         <v>18</v>
       </c>
@@ -1182,7 +1182,7 @@
     </row>
     <row r="32" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
-      <c r="B32" s="12"/>
+      <c r="B32" s="16"/>
       <c r="C32" s="1" t="s">
         <v>19</v>
       </c>
@@ -1203,7 +1203,7 @@
     </row>
     <row r="33" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
-      <c r="B33" s="12"/>
+      <c r="B33" s="16"/>
       <c r="C33" s="1" t="s">
         <v>20</v>
       </c>
@@ -1224,7 +1224,7 @@
     </row>
     <row r="34" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
-      <c r="B34" s="12"/>
+      <c r="B34" s="16"/>
       <c r="C34" s="10" t="s">
         <v>21</v>
       </c>
@@ -1257,48 +1257,48 @@
       <c r="K35" s="2"/>
     </row>
     <row r="36" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="13" t="s">
+      <c r="A36" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="14"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="13" t="s">
+      <c r="A37" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
       <c r="K37" s="2"/>
     </row>
     <row r="38" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="13" t="s">
+      <c r="A38" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="13"/>
       <c r="K38" s="2"/>
     </row>
     <row r="39" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1316,26 +1316,26 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B25:B29"/>
+    <mergeCell ref="B30:B34"/>
+    <mergeCell ref="A36:J36"/>
+    <mergeCell ref="A37:J37"/>
+    <mergeCell ref="A38:J38"/>
+    <mergeCell ref="A11:K11"/>
+    <mergeCell ref="A12:K12"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="A6:K6"/>
+    <mergeCell ref="A7:K7"/>
+    <mergeCell ref="A8:K8"/>
+    <mergeCell ref="A9:K9"/>
+    <mergeCell ref="A10:K10"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
-    <mergeCell ref="A6:K6"/>
-    <mergeCell ref="A7:K7"/>
-    <mergeCell ref="A8:K8"/>
-    <mergeCell ref="A9:K9"/>
-    <mergeCell ref="A10:K10"/>
-    <mergeCell ref="A11:K11"/>
-    <mergeCell ref="A12:K12"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="B15:B19"/>
-    <mergeCell ref="B20:B24"/>
-    <mergeCell ref="B25:B29"/>
-    <mergeCell ref="B30:B34"/>
-    <mergeCell ref="A36:J36"/>
-    <mergeCell ref="A37:J37"/>
-    <mergeCell ref="A38:J38"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1415,14 +1415,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B66A8C6-E24B-4B51-A1F1-E508C8FAA1B5}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="B5:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" ht="21.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="16" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="1"/>
@@ -1437,7 +1437,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
+      <c r="A2" s="16"/>
       <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
@@ -1452,7 +1452,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
+      <c r="A3" s="16"/>
       <c r="B3" s="1" t="s">
         <v>19</v>
       </c>
@@ -1467,7 +1467,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
+      <c r="A4" s="16"/>
       <c r="B4" s="1" t="s">
         <v>20</v>
       </c>
@@ -1482,7 +1482,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
+      <c r="A5" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1503,7 +1503,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" ht="21.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="16" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="1"/>
@@ -1518,7 +1518,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
+      <c r="A2" s="16"/>
       <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
@@ -1533,7 +1533,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
+      <c r="A3" s="16"/>
       <c r="B3" s="1" t="s">
         <v>19</v>
       </c>
@@ -1548,7 +1548,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
+      <c r="A4" s="16"/>
       <c r="B4" s="1" t="s">
         <v>20</v>
       </c>
@@ -1563,7 +1563,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
+      <c r="A5" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1577,7 +1577,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789202E7-97B3-4F14-BE32-A2762B5CFC82}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>

</xml_diff>